<commit_message>
fixed indexing of the NBD in L31 such that dihedral and pi-bond descriptors are correct
</commit_message>
<xml_diff>
--- a/obelix_ml_pipeline/data/ligand_representations/raw_data_processing/ligands_dft_nbd_model/clean_Rh_ligand_NBD_DFT_descriptors_v3.xlsx
+++ b/obelix_ml_pipeline/data/ligand_representations/raw_data_processing/ligands_dft_nbd_model/clean_Rh_ligand_NBD_DFT_descriptors_v3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avkalikadien\Documents\PhD\2021-2022\Janssen\obelix-ml-pipeline\obelix_ml_pipeline\data\ligand_representations\raw_data_processing\ligands_dft_nbd_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE24BC10-59D0-4A82-9E46-ABE08272AB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41ABC496-76E4-4802-BFBC-A908A5D4CD96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6459,13 +6459,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EP193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="J165" sqref="J165"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6905,7 +6905,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>146</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>162</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="4" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>172</v>
       </c>
@@ -7880,7 +7880,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>182</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="6" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>191</v>
       </c>
@@ -8532,7 +8532,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="7" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>202</v>
       </c>
@@ -8858,7 +8858,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="8" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>213</v>
       </c>
@@ -9184,7 +9184,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="9" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>223</v>
       </c>
@@ -9510,7 +9510,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="10" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>233</v>
       </c>
@@ -9833,7 +9833,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="11" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>243</v>
       </c>
@@ -10159,7 +10159,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="12" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>253</v>
       </c>
@@ -10485,7 +10485,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="13" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>264</v>
       </c>
@@ -10811,7 +10811,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="14" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>274</v>
       </c>
@@ -11137,7 +11137,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="15" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>284</v>
       </c>
@@ -11463,7 +11463,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="16" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>294</v>
       </c>
@@ -11789,7 +11789,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="17" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>305</v>
       </c>
@@ -12112,7 +12112,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="18" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>314</v>
       </c>
@@ -12549,7 +12549,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="19" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>324</v>
       </c>
@@ -12875,7 +12875,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="20" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>335</v>
       </c>
@@ -13195,7 +13195,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="21" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>345</v>
       </c>
@@ -13635,7 +13635,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="22" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>356</v>
       </c>
@@ -14075,7 +14075,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="23" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
         <v>366</v>
       </c>
@@ -14455,7 +14455,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="24" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
         <v>376</v>
       </c>
@@ -14895,7 +14895,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="25" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>386</v>
       </c>
@@ -15218,7 +15218,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="26" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
         <v>396</v>
       </c>
@@ -15658,7 +15658,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="27" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
         <v>406</v>
       </c>
@@ -16098,7 +16098,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="28" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
         <v>416</v>
       </c>
@@ -16538,7 +16538,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="29" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
         <v>426</v>
       </c>
@@ -16975,7 +16975,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="30" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>437</v>
       </c>
@@ -17415,7 +17415,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="31" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>447</v>
       </c>
@@ -17855,7 +17855,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="32" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
         <v>457</v>
       </c>
@@ -17884,13 +17884,13 @@
         <v>150</v>
       </c>
       <c r="J32">
-        <v>4.2494912080000002</v>
+        <v>1.40402301355782</v>
       </c>
       <c r="K32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="M32">
         <v>111</v>
@@ -17899,7 +17899,7 @@
         <v>108</v>
       </c>
       <c r="O32">
-        <v>1.524650499</v>
+        <v>1.3849718144063401</v>
       </c>
       <c r="P32" t="s">
         <v>151</v>
@@ -17914,7 +17914,7 @@
         <v>107</v>
       </c>
       <c r="T32">
-        <v>61.917755</v>
+        <v>23.124890743615399</v>
       </c>
       <c r="U32" t="s">
         <v>150</v>
@@ -17938,10 +17938,10 @@
         <v>102</v>
       </c>
       <c r="AB32">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AC32">
-        <v>-47.202822730000001</v>
+        <v>-0.44743215316303903</v>
       </c>
       <c r="AD32" t="s">
         <v>150</v>
@@ -17956,7 +17956,7 @@
         <v>152</v>
       </c>
       <c r="AH32">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="AI32">
         <v>18</v>
@@ -17965,7 +17965,7 @@
         <v>102</v>
       </c>
       <c r="AK32">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="AL32">
         <v>0.52271244900000002</v>
@@ -18178,7 +18178,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="33" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
         <v>467</v>
       </c>
@@ -18615,7 +18615,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="34" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
         <v>476</v>
       </c>
@@ -19052,7 +19052,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="35" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
         <v>485</v>
       </c>
@@ -19489,7 +19489,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="36" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
         <v>495</v>
       </c>
@@ -19926,7 +19926,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="37" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
         <v>504</v>
       </c>
@@ -20363,7 +20363,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="38" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
         <v>513</v>
       </c>
@@ -20800,7 +20800,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="39" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
         <v>522</v>
       </c>
@@ -21237,7 +21237,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="40" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
         <v>532</v>
       </c>
@@ -21674,7 +21674,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="41" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
         <v>541</v>
       </c>
@@ -22111,7 +22111,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="42" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
         <v>550</v>
       </c>
@@ -22548,7 +22548,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="43" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
         <v>560</v>
       </c>
@@ -22985,7 +22985,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="44" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
         <v>570</v>
       </c>
@@ -23422,7 +23422,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="45" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
         <v>579</v>
       </c>
@@ -23859,7 +23859,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="46" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
         <v>588</v>
       </c>
@@ -24296,7 +24296,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="47" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
         <v>597</v>
       </c>
@@ -24733,7 +24733,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="48" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
         <v>606</v>
       </c>
@@ -25170,7 +25170,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="49" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
         <v>615</v>
       </c>
@@ -25607,7 +25607,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="50" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
         <v>624</v>
       </c>
@@ -26044,7 +26044,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="51" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
         <v>633</v>
       </c>
@@ -26481,7 +26481,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="52" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="1" t="s">
         <v>643</v>
       </c>
@@ -26918,7 +26918,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="53" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="1" t="s">
         <v>652</v>
       </c>
@@ -27355,7 +27355,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="54" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="1" t="s">
         <v>661</v>
       </c>
@@ -27795,7 +27795,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="55" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="1" t="s">
         <v>671</v>
       </c>
@@ -28229,7 +28229,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="56" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="1" t="s">
         <v>680</v>
       </c>
@@ -28669,7 +28669,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="57" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="1" t="s">
         <v>690</v>
       </c>
@@ -29109,7 +29109,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="58" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="1" t="s">
         <v>700</v>
       </c>
@@ -29525,7 +29525,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="59" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="1" t="s">
         <v>712</v>
       </c>
@@ -29959,7 +29959,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="60" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="1" t="s">
         <v>723</v>
       </c>
@@ -30396,7 +30396,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="61" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="1" t="s">
         <v>732</v>
       </c>
@@ -30833,7 +30833,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="62" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="1" t="s">
         <v>743</v>
       </c>
@@ -31270,7 +31270,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="63" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="1" t="s">
         <v>753</v>
       </c>
@@ -31635,7 +31635,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="64" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="1" t="s">
         <v>761</v>
       </c>
@@ -32072,7 +32072,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="65" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="1" t="s">
         <v>770</v>
       </c>
@@ -32512,7 +32512,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="66" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="1" t="s">
         <v>780</v>
       </c>
@@ -32952,7 +32952,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="67" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="1" t="s">
         <v>790</v>
       </c>
@@ -33392,7 +33392,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="68" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="1" t="s">
         <v>800</v>
       </c>
@@ -33832,7 +33832,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="69" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="1" t="s">
         <v>810</v>
       </c>
@@ -34272,7 +34272,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="70" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="1" t="s">
         <v>820</v>
       </c>
@@ -34712,7 +34712,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="71" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="1" t="s">
         <v>830</v>
       </c>
@@ -35149,7 +35149,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="72" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="1" t="s">
         <v>839</v>
       </c>
@@ -35565,7 +35565,7 @@
         <v>848</v>
       </c>
     </row>
-    <row r="73" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="1" t="s">
         <v>849</v>
       </c>
@@ -35888,7 +35888,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="74" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="1" t="s">
         <v>859</v>
       </c>
@@ -36304,7 +36304,7 @@
         <v>868</v>
       </c>
     </row>
-    <row r="75" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="1" t="s">
         <v>869</v>
       </c>
@@ -36627,7 +36627,7 @@
         <v>878</v>
       </c>
     </row>
-    <row r="76" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="1" t="s">
         <v>879</v>
       </c>
@@ -37064,7 +37064,7 @@
         <v>887</v>
       </c>
     </row>
-    <row r="77" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="1" t="s">
         <v>888</v>
       </c>
@@ -37444,7 +37444,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="78" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="1" t="s">
         <v>897</v>
       </c>
@@ -37884,7 +37884,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="79" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="1" t="s">
         <v>907</v>
       </c>
@@ -38324,7 +38324,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="80" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="1" t="s">
         <v>917</v>
       </c>
@@ -38761,7 +38761,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="81" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="1" t="s">
         <v>927</v>
       </c>
@@ -39201,7 +39201,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="82" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="1" t="s">
         <v>937</v>
       </c>
@@ -39617,7 +39617,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="83" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="1" t="s">
         <v>947</v>
       </c>
@@ -40057,7 +40057,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="84" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="1" t="s">
         <v>957</v>
       </c>
@@ -40497,7 +40497,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="85" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="1" t="s">
         <v>968</v>
       </c>
@@ -40937,7 +40937,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="86" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="1" t="s">
         <v>978</v>
       </c>
@@ -41377,7 +41377,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="87" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="1" t="s">
         <v>988</v>
       </c>
@@ -41817,7 +41817,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="88" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="1" t="s">
         <v>999</v>
       </c>
@@ -42257,7 +42257,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="89" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="1" t="s">
         <v>1009</v>
       </c>
@@ -42697,7 +42697,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="90" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="1" t="s">
         <v>1019</v>
       </c>
@@ -43134,7 +43134,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="91" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="1" t="s">
         <v>1028</v>
       </c>
@@ -43568,7 +43568,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="92" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="1" t="s">
         <v>1037</v>
       </c>
@@ -43999,7 +43999,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="93" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="1" t="s">
         <v>1045</v>
       </c>
@@ -44430,7 +44430,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="94" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="1" t="s">
         <v>1053</v>
       </c>
@@ -44861,7 +44861,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="95" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="1" t="s">
         <v>1062</v>
       </c>
@@ -45292,7 +45292,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="96" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="1" t="s">
         <v>1070</v>
       </c>
@@ -45732,7 +45732,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="97" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="1" t="s">
         <v>1080</v>
       </c>
@@ -46163,7 +46163,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="98" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="1" t="s">
         <v>1088</v>
       </c>
@@ -46600,7 +46600,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="99" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="1" t="s">
         <v>1097</v>
       </c>
@@ -47040,7 +47040,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="100" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="1" t="s">
         <v>1107</v>
       </c>
@@ -47360,7 +47360,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="101" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="1" t="s">
         <v>1117</v>
       </c>
@@ -47794,7 +47794,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="102" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="1" t="s">
         <v>1127</v>
       </c>
@@ -48222,7 +48222,7 @@
         <v>1137</v>
       </c>
     </row>
-    <row r="103" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="1" t="s">
         <v>1138</v>
       </c>
@@ -48659,7 +48659,7 @@
         <v>1147</v>
       </c>
     </row>
-    <row r="104" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="1" t="s">
         <v>1148</v>
       </c>
@@ -49096,7 +49096,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="105" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="1" t="s">
         <v>1159</v>
       </c>
@@ -49533,7 +49533,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="106" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="1" t="s">
         <v>1169</v>
       </c>
@@ -49853,7 +49853,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="107" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="1" t="s">
         <v>1180</v>
       </c>
@@ -50290,7 +50290,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="108" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="1" t="s">
         <v>1189</v>
       </c>
@@ -50706,7 +50706,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="109" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="1" t="s">
         <v>1199</v>
       </c>
@@ -51146,7 +51146,7 @@
         <v>1208</v>
       </c>
     </row>
-    <row r="110" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="1" t="s">
         <v>1209</v>
       </c>
@@ -51586,7 +51586,7 @@
         <v>1218</v>
       </c>
     </row>
-    <row r="111" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="1" t="s">
         <v>1219</v>
       </c>
@@ -52026,7 +52026,7 @@
         <v>1229</v>
       </c>
     </row>
-    <row r="112" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="1" t="s">
         <v>1230</v>
       </c>
@@ -52466,7 +52466,7 @@
         <v>1240</v>
       </c>
     </row>
-    <row r="113" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="1" t="s">
         <v>1241</v>
       </c>
@@ -52792,7 +52792,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="114" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="1" t="s">
         <v>1251</v>
       </c>
@@ -53232,7 +53232,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="115" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" s="1" t="s">
         <v>1261</v>
       </c>
@@ -53552,7 +53552,7 @@
         <v>1179</v>
       </c>
     </row>
-    <row r="116" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A116" s="1" t="s">
         <v>1268</v>
       </c>
@@ -53872,7 +53872,7 @@
         <v>1278</v>
       </c>
     </row>
-    <row r="117" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" s="1" t="s">
         <v>1279</v>
       </c>
@@ -54303,7 +54303,7 @@
         <v>1289</v>
       </c>
     </row>
-    <row r="118" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" s="1" t="s">
         <v>1290</v>
       </c>
@@ -54740,7 +54740,7 @@
         <v>1298</v>
       </c>
     </row>
-    <row r="119" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="1" t="s">
         <v>1299</v>
       </c>
@@ -55177,7 +55177,7 @@
         <v>1307</v>
       </c>
     </row>
-    <row r="120" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" s="1" t="s">
         <v>1308</v>
       </c>
@@ -55617,7 +55617,7 @@
         <v>1317</v>
       </c>
     </row>
-    <row r="121" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" s="1" t="s">
         <v>1318</v>
       </c>
@@ -56054,7 +56054,7 @@
         <v>1326</v>
       </c>
     </row>
-    <row r="122" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" s="1" t="s">
         <v>1327</v>
       </c>
@@ -56494,7 +56494,7 @@
         <v>1336</v>
       </c>
     </row>
-    <row r="123" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" s="1" t="s">
         <v>1337</v>
       </c>
@@ -56931,7 +56931,7 @@
         <v>1345</v>
       </c>
     </row>
-    <row r="124" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" s="1" t="s">
         <v>1346</v>
       </c>
@@ -57368,7 +57368,7 @@
         <v>1355</v>
       </c>
     </row>
-    <row r="125" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" s="1" t="s">
         <v>1356</v>
       </c>
@@ -57790,7 +57790,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="126" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" s="1" t="s">
         <v>1366</v>
       </c>
@@ -58227,7 +58227,7 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="127" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" s="1" t="s">
         <v>1375</v>
       </c>
@@ -58667,7 +58667,7 @@
         <v>1384</v>
       </c>
     </row>
-    <row r="128" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" s="1" t="s">
         <v>1385</v>
       </c>
@@ -59083,7 +59083,7 @@
         <v>1394</v>
       </c>
     </row>
-    <row r="129" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" s="1" t="s">
         <v>1395</v>
       </c>
@@ -59520,7 +59520,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="130" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" s="1" t="s">
         <v>1405</v>
       </c>
@@ -59957,7 +59957,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="131" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" s="1" t="s">
         <v>1414</v>
       </c>
@@ -60394,7 +60394,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="132" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" s="1" t="s">
         <v>1423</v>
       </c>
@@ -60834,7 +60834,7 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="133" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" s="1" t="s">
         <v>1433</v>
       </c>
@@ -61253,7 +61253,7 @@
         <v>1442</v>
       </c>
     </row>
-    <row r="134" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" s="1" t="s">
         <v>1443</v>
       </c>
@@ -61690,7 +61690,7 @@
         <v>1451</v>
       </c>
     </row>
-    <row r="135" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="1" t="s">
         <v>1452</v>
       </c>
@@ -62127,7 +62127,7 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="136" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" s="1" t="s">
         <v>1461</v>
       </c>
@@ -62564,7 +62564,7 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="137" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" s="1" t="s">
         <v>1470</v>
       </c>
@@ -63001,7 +63001,7 @@
         <v>1479</v>
       </c>
     </row>
-    <row r="138" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" s="1" t="s">
         <v>1480</v>
       </c>
@@ -63438,7 +63438,7 @@
         <v>1489</v>
       </c>
     </row>
-    <row r="139" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" s="1" t="s">
         <v>1490</v>
       </c>
@@ -63878,7 +63878,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="140" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" s="1" t="s">
         <v>1501</v>
       </c>
@@ -64315,7 +64315,7 @@
         <v>1509</v>
       </c>
     </row>
-    <row r="141" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A141" s="1" t="s">
         <v>1510</v>
       </c>
@@ -64632,7 +64632,7 @@
         <v>1519</v>
       </c>
     </row>
-    <row r="142" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" s="1" t="s">
         <v>1520</v>
       </c>
@@ -64955,7 +64955,7 @@
         <v>1529</v>
       </c>
     </row>
-    <row r="143" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" s="1" t="s">
         <v>1530</v>
       </c>
@@ -65395,7 +65395,7 @@
         <v>1539</v>
       </c>
     </row>
-    <row r="144" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" s="1" t="s">
         <v>1540</v>
       </c>
@@ -65835,7 +65835,7 @@
         <v>1549</v>
       </c>
     </row>
-    <row r="145" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" s="1" t="s">
         <v>1550</v>
       </c>
@@ -66158,7 +66158,7 @@
         <v>1558</v>
       </c>
     </row>
-    <row r="146" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" s="1" t="s">
         <v>1559</v>
       </c>
@@ -66595,7 +66595,7 @@
         <v>1567</v>
       </c>
     </row>
-    <row r="147" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" s="1" t="s">
         <v>1568</v>
       </c>
@@ -67008,7 +67008,7 @@
         <v>1576</v>
       </c>
     </row>
-    <row r="148" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" s="1" t="s">
         <v>1577</v>
       </c>
@@ -67445,7 +67445,7 @@
         <v>1585</v>
       </c>
     </row>
-    <row r="149" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" s="1" t="s">
         <v>1586</v>
       </c>
@@ -67882,7 +67882,7 @@
         <v>1594</v>
       </c>
     </row>
-    <row r="150" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" s="1" t="s">
         <v>1595</v>
       </c>
@@ -68319,7 +68319,7 @@
         <v>1603</v>
       </c>
     </row>
-    <row r="151" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" s="1" t="s">
         <v>1604</v>
       </c>
@@ -68732,7 +68732,7 @@
         <v>1615</v>
       </c>
     </row>
-    <row r="152" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" s="1" t="s">
         <v>1616</v>
       </c>
@@ -69052,7 +69052,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="153" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" s="1" t="s">
         <v>1626</v>
       </c>
@@ -69375,7 +69375,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="154" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" s="1" t="s">
         <v>1636</v>
       </c>
@@ -69815,7 +69815,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="155" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" s="1" t="s">
         <v>1645</v>
       </c>
@@ -70138,7 +70138,7 @@
         <v>1654</v>
       </c>
     </row>
-    <row r="156" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="1" t="s">
         <v>1655</v>
       </c>
@@ -70464,7 +70464,7 @@
         <v>1663</v>
       </c>
     </row>
-    <row r="157" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" s="1" t="s">
         <v>1664</v>
       </c>
@@ -70784,7 +70784,7 @@
         <v>1672</v>
       </c>
     </row>
-    <row r="158" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1" t="s">
         <v>1673</v>
       </c>
@@ -71221,7 +71221,7 @@
         <v>1681</v>
       </c>
     </row>
-    <row r="159" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" s="1" t="s">
         <v>1682</v>
       </c>
@@ -71631,7 +71631,7 @@
         <v>1692</v>
       </c>
     </row>
-    <row r="160" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" s="1" t="s">
         <v>1693</v>
       </c>
@@ -72068,7 +72068,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="161" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" s="1" t="s">
         <v>1702</v>
       </c>
@@ -72505,7 +72505,7 @@
         <v>1701</v>
       </c>
     </row>
-    <row r="162" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="1" t="s">
         <v>1709</v>
       </c>
@@ -72921,7 +72921,7 @@
         <v>1718</v>
       </c>
     </row>
-    <row r="163" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" s="1" t="s">
         <v>1719</v>
       </c>
@@ -73337,7 +73337,7 @@
         <v>1728</v>
       </c>
     </row>
-    <row r="164" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="1" t="s">
         <v>1729</v>
       </c>
@@ -73777,7 +73777,7 @@
         <v>1738</v>
       </c>
     </row>
-    <row r="165" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" s="1" t="s">
         <v>1739</v>
       </c>
@@ -74199,7 +74199,7 @@
         <v>1747</v>
       </c>
     </row>
-    <row r="166" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" s="1" t="s">
         <v>1748</v>
       </c>
@@ -74636,7 +74636,7 @@
         <v>1756</v>
       </c>
     </row>
-    <row r="167" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="1" t="s">
         <v>1757</v>
       </c>
@@ -75052,7 +75052,7 @@
         <v>1766</v>
       </c>
     </row>
-    <row r="168" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A168" s="1" t="s">
         <v>1767</v>
       </c>
@@ -75492,7 +75492,7 @@
         <v>1776</v>
       </c>
     </row>
-    <row r="169" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="1" t="s">
         <v>1777</v>
       </c>
@@ -75932,7 +75932,7 @@
         <v>1787</v>
       </c>
     </row>
-    <row r="170" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="1" t="s">
         <v>1788</v>
       </c>
@@ -76372,7 +76372,7 @@
         <v>1798</v>
       </c>
     </row>
-    <row r="171" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" s="1" t="s">
         <v>1799</v>
       </c>
@@ -76809,7 +76809,7 @@
         <v>1808</v>
       </c>
     </row>
-    <row r="172" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" s="1" t="s">
         <v>1809</v>
       </c>
@@ -77249,7 +77249,7 @@
         <v>1818</v>
       </c>
     </row>
-    <row r="173" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" s="1" t="s">
         <v>1819</v>
       </c>
@@ -77689,7 +77689,7 @@
         <v>1829</v>
       </c>
     </row>
-    <row r="174" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" s="1" t="s">
         <v>1830</v>
       </c>
@@ -78105,7 +78105,7 @@
         <v>1839</v>
       </c>
     </row>
-    <row r="175" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="1" t="s">
         <v>1840</v>
       </c>
@@ -78428,7 +78428,7 @@
         <v>1848</v>
       </c>
     </row>
-    <row r="176" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" s="1" t="s">
         <v>1849</v>
       </c>
@@ -78748,7 +78748,7 @@
         <v>1857</v>
       </c>
     </row>
-    <row r="177" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1" t="s">
         <v>1858</v>
       </c>
@@ -79068,7 +79068,7 @@
         <v>1866</v>
       </c>
     </row>
-    <row r="178" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="1" t="s">
         <v>1867</v>
       </c>
@@ -79502,7 +79502,7 @@
         <v>1875</v>
       </c>
     </row>
-    <row r="179" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="1" t="s">
         <v>1876</v>
       </c>
@@ -79939,7 +79939,7 @@
         <v>1884</v>
       </c>
     </row>
-    <row r="180" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1" t="s">
         <v>1885</v>
       </c>
@@ -80352,7 +80352,7 @@
         <v>1893</v>
       </c>
     </row>
-    <row r="181" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="1" t="s">
         <v>1894</v>
       </c>
@@ -80678,7 +80678,7 @@
         <v>1903</v>
       </c>
     </row>
-    <row r="182" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="1" t="s">
         <v>1904</v>
       </c>
@@ -81004,7 +81004,7 @@
         <v>1913</v>
       </c>
     </row>
-    <row r="183" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="1" t="s">
         <v>1914</v>
       </c>
@@ -81330,7 +81330,7 @@
         <v>1924</v>
       </c>
     </row>
-    <row r="184" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="1" t="s">
         <v>1925</v>
       </c>
@@ -81770,7 +81770,7 @@
         <v>1934</v>
       </c>
     </row>
-    <row r="185" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1" t="s">
         <v>1935</v>
       </c>
@@ -82186,7 +82186,7 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="186" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="1" t="s">
         <v>1946</v>
       </c>
@@ -82599,7 +82599,7 @@
         <v>1956</v>
       </c>
     </row>
-    <row r="187" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="1" t="s">
         <v>1957</v>
       </c>
@@ -83039,7 +83039,7 @@
         <v>1966</v>
       </c>
     </row>
-    <row r="188" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="1" t="s">
         <v>1967</v>
       </c>
@@ -83476,7 +83476,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="189" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="1" t="s">
         <v>1976</v>
       </c>
@@ -83802,7 +83802,7 @@
         <v>1985</v>
       </c>
     </row>
-    <row r="190" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="1" t="s">
         <v>1986</v>
       </c>
@@ -84242,7 +84242,7 @@
         <v>1995</v>
       </c>
     </row>
-    <row r="191" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="1" t="s">
         <v>1996</v>
       </c>
@@ -84682,7 +84682,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="192" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="1" t="s">
         <v>2006</v>
       </c>
@@ -85116,7 +85116,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="193" spans="1:146" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:146" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="1" t="s">
         <v>2015</v>
       </c>

</xml_diff>